<commit_message>
Final changes, addressed all notes
</commit_message>
<xml_diff>
--- a/Daily updates.xlsx
+++ b/Daily updates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>Self Learning: Continuing with the asp.net mvc course on pluralsight</t>
+  </si>
+  <si>
+    <t>4 Hours</t>
+  </si>
+  <si>
+    <t>Self Learning: Watched videos on try catches in sql and transactions in sql, also watched videos on Delegates in c# and Eventhandlers</t>
+  </si>
+  <si>
+    <t>4.5 hours</t>
+  </si>
+  <si>
+    <t>Task: Updated the database procedures with try catch blocks and added transactions there, also added a new table that has a dataState value in it for updates etc, implemented the refresh on the controller side and hooked an event to it so that the UI can listen to that, removed transactions from the db class</t>
   </si>
 </sst>
 </file>
@@ -451,7 +463,7 @@
   <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,12 +616,26 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="3">
+        <v>44453</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="3">
+        <v>44453</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>

</xml_diff>

<commit_message>
Updated the thread to be a background thread
</commit_message>
<xml_diff>
--- a/Daily updates.xlsx
+++ b/Daily updates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Task: Addressed the comments, used threads instead of timer, applied languages to questions type, changed valdiation implementation</t>
+  </si>
+  <si>
+    <t>Self learning: Watched a couple of crash courses on asp.net mvc and continued with the pluralsight course</t>
+  </si>
+  <si>
+    <t>Task: worked on the end user documentataion</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
   <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,12 +697,26 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="3">
+        <v>44458</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="3">
+        <v>44458</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>

</xml_diff>